<commit_message>
Add value 'Information not provided' on register when no values are provided in XML
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2018_register_model_20181114.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2018_register_model_20181114.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="17" r:id="rId1"/>
@@ -6935,6 +6935,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7011,6 +7012,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -7034,6 +7036,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -7041,12 +7044,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD59CE5F-E8D6-4FE0-AC79-15942F8E00A2}" type="CELLRANGE">
+                    <a:fld id="{72F167E5-6F77-4E9F-8DBC-7E8F484B4F29}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -7064,6 +7068,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -7072,12 +7077,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{039E247E-CBB7-4FDD-BD73-D2CE5F368ED5}" type="CELLRANGE">
+                    <a:fld id="{DC2A6DC7-ED23-4135-8B94-BD512455A395}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -7095,6 +7101,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -7140,6 +7147,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -7246,6 +7254,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -7269,6 +7278,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -7276,12 +7286,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E0FED6E8-EC7A-4912-933A-C35361639473}" type="CELLRANGE">
+                    <a:fld id="{41D83162-3D47-4E26-B033-AAC21FDAAD7D}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -7299,6 +7310,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -7307,12 +7319,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{54B29DA5-E95D-4806-88E6-8519914AF4AD}" type="CELLRANGE">
+                    <a:fld id="{E3F4294C-1E51-4CF6-902B-F8DC6110277B}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -7330,6 +7343,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -7375,6 +7389,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -7549,6 +7564,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10611,6 +10627,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13088,6 +13105,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13559,6 +13577,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -13633,6 +13652,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13744,6 +13764,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13820,6 +13841,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -13843,6 +13865,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -13879,6 +13902,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -13886,12 +13910,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69C9A033-B380-4E57-A46E-75923C00119C}" type="CELLRANGE">
+                    <a:fld id="{F8832AA4-5B56-435B-A59D-95365AA8597D}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -13909,6 +13934,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -13954,6 +13980,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -14060,6 +14087,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -14083,6 +14111,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -14090,12 +14119,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FCCE6A2C-3521-4B40-B431-510D0A1C6886}" type="CELLRANGE">
+                    <a:fld id="{97151696-6E4A-4AAB-ADBA-A16F7EE3CEC5}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -14113,6 +14143,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -14121,12 +14152,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D25B349B-5491-4838-B28A-4375F93B9CAD}" type="CELLRANGE">
+                    <a:fld id="{E9A2E351-5B19-42DC-BFA8-C3321FC56D0F}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -14144,6 +14176,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -14189,6 +14222,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -14312,6 +14346,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15166,6 +15201,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15466,6 +15502,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15542,12 +15579,13 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8500997F-8179-4688-8AB6-9DE1ABA46F90}" type="CELLRANGE">
+                    <a:fld id="{65CFF619-B734-4375-A7F2-13A893CA2DA9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -15565,6 +15603,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -15572,12 +15611,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AB8456DB-1C1F-4082-9FB0-493CA9C575D5}" type="CELLRANGE">
+                    <a:fld id="{2608A3D5-23AB-4714-987F-E1E1BBF15D3B}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -15595,6 +15635,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -15603,12 +15644,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E4A0017B-6553-4F77-858A-95F61FBCBC2C}" type="CELLRANGE">
+                    <a:fld id="{E4AA8959-4CE6-4859-9C86-F84BB85E67B0}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -15626,6 +15668,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -15671,6 +15714,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -15777,12 +15821,13 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5780403-192E-4BA5-BB59-BA8077F88203}" type="CELLRANGE">
+                    <a:fld id="{919A5EBF-57C0-4191-AC2F-6FC7B04677DF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -15800,6 +15845,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -15807,12 +15853,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B056855D-44D5-42D6-8F02-5307F420EE93}" type="CELLRANGE">
+                    <a:fld id="{2957BE6D-DDF5-4DCE-8877-21FC199C3CC8}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -15830,6 +15877,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -15838,12 +15886,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{57CBE8D5-B532-4D7C-843E-D0AE246E21FA}" type="CELLRANGE">
+                    <a:fld id="{A4954806-2AE9-427D-A032-E970B32AAF7D}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -15861,6 +15910,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -15906,6 +15956,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -16080,6 +16131,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16275,6 +16327,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16351,6 +16404,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -16374,6 +16428,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -16381,12 +16436,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FE3A56C4-F93A-44B3-91ED-EE80F7263483}" type="CELLRANGE">
+                    <a:fld id="{F1A57023-FCC4-4159-8C8D-5AB0288F6D7C}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -16404,6 +16460,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -16412,12 +16469,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{694D3D22-9069-4552-BDAD-797BD96C425B}" type="CELLRANGE">
+                    <a:fld id="{953AB43F-C57C-491B-8DFD-5B4F2B78B332}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -16435,6 +16493,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -16480,6 +16539,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -16586,6 +16646,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -16609,6 +16670,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -16616,12 +16678,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0423C93F-85A5-49FF-8A70-4A7B6D835BA4}" type="CELLRANGE">
+                    <a:fld id="{C946EB70-B41D-43E9-82A4-5F5BBF3D9089}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -16639,6 +16702,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -16647,12 +16711,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A64C859-B548-4666-A48B-CB67074AFCCF}" type="CELLRANGE">
+                    <a:fld id="{6D5EF732-3C9C-4439-8A92-DA64622F5C32}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -16670,6 +16735,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -16715,6 +16781,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -16838,6 +16905,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -17143,6 +17211,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17506,6 +17575,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -20090,6 +20160,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20320,7 +20391,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -20524,6 +20597,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20914,6 +20988,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -21034,6 +21109,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -21225,6 +21301,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21588,6 +21665,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -21893,6 +21971,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -22256,6 +22335,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -22566,6 +22646,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23067,6 +23148,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -41713,7 +41795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -42393,7 +42475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG178"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -46874,7 +46956,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48227,11 +48309,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CV51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="CB5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" sqref="A1:B4"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>